<commit_message>
added file creation script
</commit_message>
<xml_diff>
--- a/public/excel/food.xlsx
+++ b/public/excel/food.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjwinklejmj/WORKSPACE/Italian_Hamilton/public/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A72405E-9ACF-5B4F-AE10-0A6FCEC31648}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCF0555-5240-074D-B398-35050E5C9DE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2140" yWindow="1400" windowWidth="29340" windowHeight="17440" xr2:uid="{934A5C47-FC82-BC4D-9400-638888CABA05}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="148">
   <si>
     <t>ITALIAN</t>
   </si>
@@ -457,6 +457,27 @@
   </si>
   <si>
     <t>l'arancia</t>
+  </si>
+  <si>
+    <t>la mandorla</t>
+  </si>
+  <si>
+    <t>la salsa di mele</t>
+  </si>
+  <si>
+    <t>sauce</t>
+  </si>
+  <si>
+    <t>la salsa</t>
+  </si>
+  <si>
+    <t>il carciofo</t>
+  </si>
+  <si>
+    <t>l'asparago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noun </t>
   </si>
 </sst>
 </file>
@@ -817,14 +838,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0549DD43-98DE-DC4F-B0DD-B69F47AA9087}">
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="G105" sqref="G105"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -846,6 +868,9 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -857,6 +882,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -868,6 +896,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -879,6 +910,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -2245,7 +2279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>132</v>
       </c>
@@ -2256,7 +2290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>133</v>
       </c>
@@ -2267,7 +2301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>134</v>
       </c>
@@ -2278,7 +2312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>135</v>
       </c>
@@ -2289,7 +2323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>136</v>
       </c>
@@ -2300,7 +2334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>137</v>
       </c>
@@ -2311,7 +2345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>138</v>
       </c>
@@ -2319,6 +2353,20 @@
         <v>139</v>
       </c>
       <c r="D135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>144</v>
+      </c>
+      <c r="B136" t="s">
+        <v>143</v>
+      </c>
+      <c r="C136" t="s">
+        <v>147</v>
+      </c>
+      <c r="D136" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>